<commit_message>
deleted:    org/reference/.#2020-09-07_reference.org 	modified:   org/reference/2020-09-07_reference.org 	new file:   org/reference/2020-09-08_reference.org 	new file:   org/reference/2020-09-09_reference.org 	new file:   org/reference/2020-09-10_reference.org 	new file:   org/reference/2020-09-12_reference.org 	new file:   org/reference/2020-09-13_reference.org 	new file:   org/reference/data/6c/607b80-7a06-48a6-8f7a-16a36099de25/file-to-gmail-2012.sh 	modified:   告発状項目一覧.xlsx
update 2020-09-13_1634 a66-XTe
</commit_message>
<xml_diff>
--- a/告発状項目一覧.xlsx
+++ b/告発状項目一覧.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="104">
   <si>
     <t xml:space="preserve">済</t>
   </si>
@@ -79,7 +79,25 @@
     <t xml:space="preserve">松浦さんの愛人の息子として入社した被告発人安田繁克（平成元年9月？）</t>
   </si>
   <si>
+    <t xml:space="preserve">ほぼ同じ頃に入社した西口君と名古屋の元暴力団員S藤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長く勘違いしていた，入社のきっかけとなった被告発人安田繁克の母親の愛人</t>
+  </si>
+  <si>
     <t xml:space="preserve">被告発人安田繁克と被告発人大網健二との接点（平成2年春か秋）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宇出津のK村さんと姫のNさんという被告発人大網健二と市場急配センターの接点</t>
+  </si>
+  <si>
+    <t xml:space="preserve">被害者安藤文さんを市場急配センターに紹介したともされる，笹田君と峰田君</t>
+  </si>
+  <si>
+    <t xml:space="preserve">笹田君と被告発人大網健二の中古車販売を巡るトラブル</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中古のBMW</t>
   </si>
   <si>
     <t xml:space="preserve">平成3年6月，被害者安藤文さんに電話で言われた，どちらの安田</t>
@@ -330,6 +348,7 @@
       <color rgb="FF000000"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -352,18 +371,21 @@
       <color rgb="FFA7074B"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="游ゴシック"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -420,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -439,10 +461,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -526,19 +544,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="8:15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="130.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="67.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="132.75"/>
   </cols>
   <sheetData>
@@ -563,7 +581,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -580,7 +598,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -597,7 +615,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -614,7 +632,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -631,7 +649,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -648,7 +666,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -665,7 +683,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -682,9 +700,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="0" t="s">
         <v>15</v>
       </c>
@@ -695,14 +711,32 @@
         <v>17</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -715,254 +749,258 @@
         <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>22</v>
+      <c r="F13" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>23</v>
+      <c r="F14" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>24</v>
+      <c r="F15" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>25</v>
+      <c r="E16" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="E17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="F18" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>28</v>
+      <c r="E19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="0" t="s">
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="0" t="s">
@@ -972,72 +1010,65 @@
         <v>16</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E25" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="6"/>
+      <c r="E26" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>37</v>
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>38</v>
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="0" t="s">
@@ -1047,14 +1078,14 @@
         <v>16</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="0" t="s">
@@ -1064,65 +1095,72 @@
         <v>16</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="0" t="s">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="0" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="0" t="s">
@@ -1137,12 +1175,9 @@
       <c r="E34" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="0" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="0" t="s">
@@ -1155,599 +1190,593 @@
         <v>45</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="0" t="s">
+    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="E37" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="0" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="E38" s="0" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="6" t="s">
+    <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="6" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="6" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F41" s="6" t="s">
+      <c r="E41" s="0" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" s="6" t="s">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F43" s="6" t="s">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="E43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F44" s="6" t="s">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>60</v>
       </c>
+      <c r="F44" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E45" s="6" t="s">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="6" t="s">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F47" s="6" t="s">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F48" s="6" t="s">
+      <c r="A48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F49" s="6" t="s">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F50" s="6" t="s">
+      <c r="C50" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="E50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="0" t="s">
+      <c r="C51" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="F51" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="0" t="s">
+      <c r="C52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E52" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="0" t="s">
+      <c r="F52" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" s="0" t="s">
+      <c r="C53" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E53" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F53" s="0" t="s">
+      <c r="F53" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="0" t="s">
+      <c r="C54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E54" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F54" s="0" t="s">
+      <c r="F54" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="0" t="s">
+      <c r="C55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E55" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E56" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="E57" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F57" s="0" t="s">
+      <c r="E58" s="0" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E58" s="0" t="s">
+      <c r="F58" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F58" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="E59" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F59" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="E60" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F62" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E63" s="0" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="F63" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E64" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F64" s="0" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E66" s="0" t="s">
         <v>84</v>
@@ -1757,17 +1786,17 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>84</v>
@@ -1777,17 +1806,17 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>84</v>
@@ -1797,14 +1826,14 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>88</v>
@@ -1814,160 +1843,254 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>88</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F70" s="0" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>88</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>88</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>88</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F74" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D75" s="0" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>95</v>
       </c>
+      <c r="F75" s="0" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>95</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>95</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>